<commit_message>
update: rlabels and Code Presence Matrices
</commit_message>
<xml_diff>
--- a/SSM-websites-and-software.xlsx
+++ b/SSM-websites-and-software.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36740" yWindow="600" windowWidth="36500" windowHeight="19320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38320" yWindow="-460" windowWidth="38400" windowHeight="22720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DataProcSeqAndProcesses" sheetId="3" r:id="rId1"/>
     <sheet name="SSMWebsites" sheetId="1" r:id="rId2"/>
     <sheet name="ToDo" sheetId="2" r:id="rId3"/>
     <sheet name="Documents" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="179">
   <si>
     <t>URL</t>
   </si>
@@ -91,15 +92,9 @@
     <t>The single command line argument is the path to a text file of the format exported by clicking on the 'Save Text' button on http://syssci.renci.org/sort/. The result is another file with the same path except with the extension '.json' that contains a JSON object equivalent to what you would have gotten if you'd clicked on the 'Save JSON' button. See https://github.com/steve9000gi/sort for details.</t>
   </si>
   <si>
-    <t>https://github.com/steve9000gi/text2JSON</t>
-  </si>
-  <si>
     <t>text2JSON.py path_to_text_file</t>
   </si>
   <si>
-    <t>https://github.com/steve9000gi/add_codes_to_SSMs</t>
-  </si>
-  <si>
     <t>add_codes_to_SSMs.py ssm_dir cblm_dir cssm_dir</t>
   </si>
   <si>
@@ -136,13 +131,7 @@
     <t>https://github.com/steve9000gi/ssm/tree/mental-health-in-schools</t>
   </si>
   <si>
-    <t>https://github.com/steve9000gi/create_code_matrices</t>
-  </si>
-  <si>
     <t>create_code_matrices.py cblm_dir code_matrix_dir</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/get_mental_maps</t>
   </si>
   <si>
     <t>get_mental_maps.py output_directory</t>
@@ -402,27 +391,15 @@
     <t>https://github.com/steve9000gi/sort/blob/master/README.md</t>
   </si>
   <si>
-    <t>https://github.com/steve9000gi/text2JSON/blob/master/README.md</t>
-  </si>
-  <si>
     <t>https://github.com/steve9000gi/AddCodesToBLM/blob/master/README.md</t>
   </si>
   <si>
-    <t>https://github.com/steve9000gi/create_code_matrices/blob/master/README.md</t>
-  </si>
-  <si>
     <t>Also the README.md files in the various SSM-related GitHub repos:</t>
   </si>
   <si>
     <t>https://github.com/steve9000gi/extractMaps/blob/master/README.md</t>
   </si>
   <si>
-    <t>https://github.com/steve9000gi/get_mental_maps/blob/master/README.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/add_codes_to_SSMs/blob/master/README.md</t>
-  </si>
-  <si>
     <t>Text-only example runthrough : SSMs -&gt; BLMS -&gt; sort -&gt; CBLM -&gt; CM and CPM</t>
   </si>
   <si>
@@ -468,9 +445,6 @@
     <t xml:space="preserve">In use? </t>
   </si>
   <si>
-    <t>Draft TitleX questions need to be updated</t>
-  </si>
-  <si>
     <t>For "Role" only</t>
   </si>
   <si>
@@ -492,9 +466,6 @@
     <t>ALL (type only displayed for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
   </si>
   <si>
-    <t>Version/ Timestamp</t>
-  </si>
-  <si>
     <t>8/15/2017:</t>
   </si>
   <si>
@@ -556,6 +527,109 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>"ssm"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard-TitleV"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard-d (/?module=CaregiversOfCYSHCN)"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard-TitleX"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard"</t>
+  </si>
+  <si>
+    <t>Version/Timestamp</t>
+  </si>
+  <si>
+    <t>Draft TitleX questions need to be updated. Also awaiting general review of user interface.</t>
+  </si>
+  <si>
+    <t>add_rlabels_to_SSMs</t>
+  </si>
+  <si>
+    <t>add_rlabels_to_SSMs.py. An "rlabel" is a string that uniquely identifies a Responsibility node in the context of a set (a directory) of System Support Maps (SSMs). Treat each Responsibility node as the root of a graph comprised of all the nodes that are linked to it in the SSM to which it belongs. Traverse that graph, attaching to each node the rlabel that uniquely identifies the root Responsibility.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing</t>
+  </si>
+  <si>
+    <t>add_rlabels_to_SSMs.py indir outdir [use_full_filename] [undir]</t>
+  </si>
+  <si>
+    <t>CMs_to_3cols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMs_to_3cols.py: Reads in a directory of code matrices (CMs). Outputs a directory of "3cols," which are 2D arrays, each arranged in three columns, thusly:   
+from to value   
+where "from" and "to" are codes, and "value" is the number of edges in the originating set of SSMs that go from "from" to "to." In each 3cols file output there is a row for each element in its corresponding CM.   </t>
+  </si>
+  <si>
+    <t>CMs_to_3cols.py cm_dir output_dir [min_val]</t>
+  </si>
+  <si>
+    <t>Miscellaneous scripts</t>
+  </si>
+  <si>
+    <t>get_maps_by_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_maps_by_version.py: Retrieve and write as .json files all the system support maps (ssms) from the ssm database that have a "version" value in   
+the "document" field that matches command line argument "version." </t>
+  </si>
+  <si>
+    <t>get_maps_by_version.py version output_directory</t>
+  </si>
+  <si>
+    <t>get_NY_maps_with_demo</t>
+  </si>
+  <si>
+    <t>get_NY_maps_with_demo.py: Retrieve and write as .json files all the system support maps (ssms) from the ssm database that have a "state" key in  
+the "document" field and where the associated value is "NY".</t>
+  </si>
+  <si>
+    <t>get_NY_maps_with_demo.py output_directory</t>
+  </si>
+  <si>
+    <t>get_reg_info</t>
+  </si>
+  <si>
+    <t>get_reg_info.py: get registration info for each user associated with one or more of a directory of system support maps.</t>
+  </si>
+  <si>
+    <t>get_reg_info in_dir out_fname</t>
+  </si>
+  <si>
+    <t>get_ssm_demographics</t>
+  </si>
+  <si>
+    <t>get_ssm_demographics.py: Read a directory of ssms, write out their demographic info to a csv file called demographics.csv.</t>
+  </si>
+  <si>
+    <t>get_ssm_demographics.py in_dir</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-add_codes_to_ssms.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/add_rlabels_to_SSMs.py</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-create_code_matrices.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-get_maps_by_version.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-get_mental_maps.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-text2JSON.md</t>
   </si>
 </sst>
 </file>
@@ -563,7 +637,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -759,7 +833,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="34">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -794,8 +868,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -883,12 +983,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -981,6 +1075,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="30"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -993,15 +1094,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="30"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="34">
+  <cellStyles count="60">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1027,6 +1122,32 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
@@ -1057,13 +1178,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>189991</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2196157</xdr:rowOff>
+      <xdr:rowOff>2006165</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1073,15 +1194,21 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="11696700" cy="7047557"/>
+          <a:off x="0" y="189991"/>
+          <a:ext cx="11696700" cy="6667574"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1415,19 +1542,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="32"/>
-    <col min="2" max="2" width="16.83203125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="91.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="32" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="32"/>
+    <col min="1" max="1" width="8.83203125" style="30"/>
+    <col min="2" max="2" width="18.1640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="91.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="382" customHeight="1"/>
@@ -1437,7 +1565,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>1</v>
@@ -1449,7 +1577,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G4" s="22"/>
     </row>
@@ -1458,10 +1586,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>16</v>
@@ -1470,16 +1598,16 @@
         <v>19</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="28" customFormat="1" ht="120">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="28" customFormat="1" ht="96">
       <c r="A6" s="24">
         <f t="shared" ref="A6:A11" si="0">A5+1</f>
         <v>2</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>17</v>
@@ -1488,32 +1616,32 @@
         <v>20</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:7" s="28" customFormat="1" ht="48">
+    <row r="7" spans="1:7" s="28" customFormat="1" ht="36">
       <c r="A7" s="24">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G7" s="29"/>
     </row>
@@ -1523,19 +1651,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>24</v>
+        <v>155</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G8" s="29"/>
     </row>
@@ -1545,41 +1673,41 @@
         <v>5</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G9" s="29"/>
     </row>
-    <row r="10" spans="1:7" s="28" customFormat="1" ht="60">
+    <row r="10" spans="1:7" s="28" customFormat="1" ht="36">
       <c r="A10" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>37</v>
+        <v>155</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G10" s="29"/>
     </row>
@@ -1589,29 +1717,160 @@
         <v>7</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="E11" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="25" t="s">
-        <v>44</v>
-      </c>
       <c r="G11" s="29"/>
     </row>
-    <row r="12" spans="1:7" s="28" customFormat="1">
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="29"/>
+    <row r="12" spans="1:7" s="28" customFormat="1" ht="82" customHeight="1">
+      <c r="A12" s="24">
+        <v>8</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" ht="93" customHeight="1">
+      <c r="A13" s="24">
+        <v>9</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="70" customFormat="1">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="36">
+      <c r="A15" s="24">
+        <v>10</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="36">
+      <c r="A16" s="24">
+        <v>11</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="24">
+      <c r="A17" s="24">
+        <v>12</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="24">
+      <c r="A18" s="24">
+        <v>13</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1632,9 +1891,9 @@
   </sheetPr>
   <dimension ref="A1:O217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1648,7 +1907,7 @@
     <col min="8" max="9" width="27" style="8" customWidth="1"/>
     <col min="10" max="10" width="19.33203125" style="6" customWidth="1"/>
     <col min="11" max="11" width="14.83203125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" style="6" customWidth="1"/>
     <col min="13" max="13" width="18.5" style="5" customWidth="1"/>
     <col min="14" max="14" width="27.6640625" style="5" customWidth="1"/>
     <col min="15" max="15" width="31.1640625" style="5" customWidth="1"/>
@@ -1673,45 +1932,45 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:15" s="60" customFormat="1" ht="120">
-      <c r="A2" s="57" t="s">
+    <row r="2" spans="1:15" s="58" customFormat="1" ht="120">
+      <c r="A2" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="58" t="s">
+      <c r="D2" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="58" t="s">
+      <c r="F2" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="M2" s="58" t="s">
-        <v>68</v>
+      <c r="I2" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="M2" s="56" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="60">
@@ -1722,37 +1981,37 @@
         <v>3</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>61</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="140">
@@ -1764,41 +2023,41 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>61</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="59" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N4" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="O4" s="42" t="s">
-        <v>84</v>
+        <v>61</v>
+      </c>
+      <c r="N4" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="40">
@@ -1806,34 +2065,34 @@
         <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="38" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="D5" s="62"/>
+      <c r="E5" s="36" t="s">
+        <v>31</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="10" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="40" t="s">
-        <v>63</v>
+        <v>84</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>59</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" s="61" t="s">
-        <v>13</v>
+        <v>59</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>150</v>
       </c>
       <c r="M5" s="14" t="s">
         <v>13</v>
@@ -1844,81 +2103,81 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="10" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="J6" s="40" t="s">
-        <v>62</v>
+        <v>84</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L6" s="61" t="s">
-        <v>13</v>
+        <v>60</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>150</v>
       </c>
       <c r="M6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="90" customHeight="1">
-      <c r="A7" s="43">
+      <c r="A7" s="41">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="43" t="s">
+      <c r="C7" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="69" t="s">
-        <v>154</v>
-      </c>
-      <c r="H7" s="46" t="s">
+      <c r="G7" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>63</v>
+      <c r="I7" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>59</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L7" s="61"/>
+        <v>59</v>
+      </c>
+      <c r="L7" s="59"/>
       <c r="M7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="O7" s="67" t="s">
-        <v>82</v>
+      <c r="N7" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="68" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="120">
@@ -1926,15 +2185,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="37" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>13</v>
@@ -1944,57 +2203,57 @@
         <v>13</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>82</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L8" s="61" t="s">
-        <v>13</v>
+        <v>59</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>148</v>
       </c>
       <c r="M8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="66"/>
-      <c r="O8" s="68"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="69"/>
     </row>
     <row r="9" spans="1:15" ht="120">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="40" t="s">
-        <v>62</v>
+        <v>86</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="59" t="s">
         <v>14</v>
       </c>
       <c r="M9" s="10" t="s">
@@ -2006,15 +2265,15 @@
         <f>A8+1</f>
         <v>7</v>
       </c>
-      <c r="B10" s="39" t="s">
-        <v>118</v>
+      <c r="B10" s="37" t="s">
+        <v>110</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>13</v>
@@ -2024,35 +2283,35 @@
         <v>13</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="J10" s="55" t="s">
-        <v>127</v>
+        <v>111</v>
+      </c>
+      <c r="J10" s="53" t="s">
+        <v>118</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="L10" s="61" t="s">
-        <v>13</v>
+        <v>112</v>
+      </c>
+      <c r="L10" s="59" t="s">
+        <v>149</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="84" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="111" customHeight="1">
       <c r="A11" s="9">
         <f>A9+1</f>
         <v>8</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>123</v>
+      <c r="B11" s="37" t="s">
+        <v>115</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="54" t="s">
-        <v>124</v>
+      <c r="E11" s="52" t="s">
+        <v>116</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>14</v>
@@ -2062,19 +2321,19 @@
         <v>13</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>62</v>
+        <v>152</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" s="61" t="s">
-        <v>13</v>
+        <v>60</v>
+      </c>
+      <c r="L11" s="59" t="s">
+        <v>147</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="120">
@@ -2082,11 +2341,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="15"/>
@@ -2098,19 +2357,19 @@
         <v>14</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J12" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>61</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="61" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="L12" s="59" t="s">
+        <v>61</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="80">
@@ -2118,39 +2377,39 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>61</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="8:9">
@@ -2971,159 +3230,159 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="37" customWidth="1"/>
-    <col min="2" max="2" width="96.83203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="96.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="33" customFormat="1">
-      <c r="A1" s="36"/>
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:4" s="31" customFormat="1">
+      <c r="A1" s="34"/>
+      <c r="B1" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45">
-      <c r="A5" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>78</v>
+      <c r="A5" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>80</v>
+      <c r="A6" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" s="53" t="s">
-        <v>112</v>
+      <c r="B8" s="51" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="35" t="s">
-        <v>113</v>
+      <c r="B10" s="33" t="s">
+        <v>105</v>
       </c>
       <c r="C10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" s="60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="61" customHeight="1">
+      <c r="A18" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14" customHeight="1">
+      <c r="A19" s="49"/>
+      <c r="B19" s="64">
+        <v>42963</v>
+      </c>
+      <c r="D19" s="49"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" s="33" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="56" t="s">
+    <row r="21" spans="1:4">
+      <c r="B21" s="33" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="B15" s="63" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="56" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="B17" s="62" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="61" customHeight="1">
-      <c r="A18" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="51" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14" customHeight="1">
-      <c r="A19" s="51"/>
-      <c r="B19" s="70">
-        <v>42963</v>
-      </c>
-      <c r="D19" s="51"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="B20" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="35" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3139,125 +3398,153 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="96.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="96.6640625" style="49" customWidth="1"/>
     <col min="2" max="2" width="104.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="46" customFormat="1">
+      <c r="A2" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="49" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="48" customFormat="1">
-      <c r="A2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="50" t="s">
+      <c r="B5" t="s">
         <v>94</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="43" customHeight="1">
+      <c r="A6" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="51" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43" customHeight="1">
-      <c r="A6" s="51" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="49" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="49" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="49" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="49" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="49" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="52" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="51" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="51" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="49" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="51" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" t="s">
-        <v>148</v>
+    <row r="20" spans="1:2">
+      <c r="A20" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A17" r:id="rId1"/>
+    <hyperlink ref="A20" r:id="rId1"/>
   </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
additional explication for Code Matrix files
</commit_message>
<xml_diff>
--- a/SSM-websites-and-software.xlsx
+++ b/SSM-websites-and-software.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevec/ssm-documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D60BE04-8A72-D141-AA91-455D0854E5B0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37440" yWindow="320" windowWidth="36540" windowHeight="21760" tabRatio="500"/>
+    <workbookView xWindow="-37360" yWindow="720" windowWidth="36540" windowHeight="21760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataProcSeqAndProcesses" sheetId="3" r:id="rId1"/>
@@ -247,8 +248,355 @@
     <t>Is there a way to redirect people that go to no longer supported wizard pages to new pages? (with a click-able link?)</t>
   </si>
   <si>
+    <t>Is it easier to put the demog survey in as a separate webpage, which when complete passes info to the wizard (advantage being that we can use the wizard site infrastructure (passing a new yaml, and a project specific demog survey and potentially project specific drop down lists, etc).</t>
+  </si>
+  <si>
+    <t>do now</t>
+  </si>
+  <si>
+    <t>Is it easy to name the .json files geog_firstPartEmail_SSMID_role.json</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>**The "Finish" button has been hidden in an effort to improve the user experience. Problem: Now, any post-wizard user changes to the map are not preserved.</t>
+  </si>
+  <si>
+    <t>Green fill means that presence or absence of drop-down lists in this version corresponds to text (no mention of drop-down lists if there aren't any).</t>
+  </si>
+  <si>
+    <t>Gray fill means this website is decommissioned, i.e., the user can't see it and is instead redirected to another website.</t>
+  </si>
+  <si>
+    <t>* Should the Qualtrics surveys be removed? Who's using them? 2017/06/05: we're keeping them and adding one for TitleX/Family Planning.</t>
+  </si>
+  <si>
+    <t>CYSHCN: fixed 2017/06/13</t>
+  </si>
+  <si>
+    <t>Demographic questions?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>state; county/municipality; race;  Hispanic?; language;  child's age; insurance; health conditions</t>
+  </si>
+  <si>
+    <t>position; grade[s]; age range; years at school;  race/ethnicity; school location</t>
+  </si>
+  <si>
+    <t>Wizard prototype (maintained for backwards compatibility). Identical to ssm-wizard-d/?module=CaregiversOfCYSHCN from the user's viewpoint. Decommissioned 2017/06/13: url redirects to http://syssci.renci.org/ssm-wizard-d/?module=CaregiversOfCYSHCN.</t>
+  </si>
+  <si>
+    <t>NA (decommissioned)</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/blob/master/SSM-websites-and-software.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/blob/master/SSM_Processing_Sequence.txt</t>
+  </si>
+  <si>
+    <t>This spreadsheet</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/blob/master/Editing_Sorted_SSM_Documents.docx</t>
+  </si>
+  <si>
+    <t>Tips for manually editing sorted text items while maximizing the likelihood of the results being processable.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/blob/master/File_Formats_for_the_Sort_Segment_of_the_System_Support_Mapping_Processing_Sequence.docx</t>
+  </si>
+  <si>
+    <t>Details of the various sort file formats with emphasis on .json.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/binary-link-matrix/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/AddCodesToBLM/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>Also the README.md files in the various SSM-related GitHub repos:</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/extractMaps/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>Text-only example runthrough : SSMs -&gt; BLMS -&gt; sort -&gt; CBLM -&gt; CM and CPM</t>
+  </si>
+  <si>
+    <t>8/10/2017 for all SSM Wizard versions:</t>
+  </si>
+  <si>
+    <t>Restore hidden ""Finish" button as "Save" (doesn't close wizard)</t>
+  </si>
+  <si>
+    <t>Fix Minimize</t>
+  </si>
+  <si>
+    <t>Enforce limits on zoom and translate</t>
+  </si>
+  <si>
+    <t>Fix completions (elements of completions objects should be arrays)</t>
+  </si>
+  <si>
+    <t>Add wizard type (e.g., TitleX or TitleV), version number, and timestamp to source and to SSM json output</t>
+  </si>
+  <si>
+    <t>http://syssci.renci.org/ssm-wizard-TitleX</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>"Finish" converted to "Save"</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/tree/wizard-TitleX</t>
+  </si>
+  <si>
+    <t>http://syssci.renci.org/ssm-wizard-TitleV</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/tree/wizard-TitleV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In use? </t>
+  </si>
+  <si>
+    <t>For "Role" only</t>
+  </si>
+  <si>
+    <t>ssm-wizard for Maternal and Child Health/Title V. Based on http://syssci.renci.org/ssm-wizard/?module=TitleVWorkforce but includes custom text and demographic questions. No text entry response dropdown completions lists.</t>
+  </si>
+  <si>
+    <t>Dropdown completions lists for text entry</t>
+  </si>
+  <si>
+    <t>ALL (done for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
+  </si>
+  <si>
+    <t>ALL (done for ssm-wizard-TitleX)</t>
+  </si>
+  <si>
+    <t>ALL (type only displayed for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
+  </si>
+  <si>
+    <t>8/15/2017:</t>
+  </si>
+  <si>
+    <t>Add wizard version (e.g., TitleX or TitleV) and timestamp to source and to SSM json output</t>
+  </si>
+  <si>
+    <t>done for ssm-wizard-TitleX, ssm-wizard-TitleV, ssm, ssm-wizard, ssm-wizard-d)</t>
+  </si>
+  <si>
+    <t>not done: mental, beh</t>
+  </si>
+  <si>
+    <t>In use by…</t>
+  </si>
+  <si>
+    <t>Fill in who is currently using each website (over time)</t>
+  </si>
+  <si>
+    <t>Fill in all docs, videos etc that support use of each version of the wizard</t>
+  </si>
+  <si>
+    <t>UIC doctoral student Kevin Borrup's "Roles in Mental Health Care within Schools in Connecticut Research Study."</t>
+  </si>
+  <si>
+    <t>Detailed guide with screenshots for parents/caregivers of CYSHN; https://www.youtube.com/channel/UCFTWoJ1iXFTqrq-62RZ68hA</t>
+  </si>
+  <si>
+    <t>done for http://syssci.renci.org/ssm-wizard-TitleX</t>
+  </si>
+  <si>
+    <t>look into [probably not. Would require passing data between websites.]</t>
+  </si>
+  <si>
+    <t>if easy [possible but not easy: requires JSON data extraction within PostgreSQL]</t>
+  </si>
+  <si>
+    <t>youtube site with instructions for the Title V SSM Wizard</t>
+  </si>
+  <si>
+    <t> https://www.youtube.com/channel/UCFTWoJ1iXFTqrq-62RZ68hA</t>
+  </si>
+  <si>
+    <t>Deanna Befus</t>
+  </si>
+  <si>
+    <t>NY State DOH caregivers</t>
+  </si>
+  <si>
+    <t>NMCHWDC Workforce; NY State DOH workforce</t>
+  </si>
+  <si>
+    <t>Larissa Calancie: Title V NMCHWDC</t>
+  </si>
+  <si>
+    <t>decommissioned</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>"ssm"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard-TitleV"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard-d (/?module=CaregiversOfCYSHCN)"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard-TitleX"</t>
+  </si>
+  <si>
+    <t>"ssm-wizard"</t>
+  </si>
+  <si>
+    <t>Version/Timestamp</t>
+  </si>
+  <si>
+    <t>Draft TitleX questions need to be updated. Also awaiting general review of user interface.</t>
+  </si>
+  <si>
+    <t>add_rlabels_to_SSMs</t>
+  </si>
+  <si>
+    <t>add_rlabels_to_SSMs.py. An "rlabel" is a string that uniquely identifies a Responsibility node in the context of a set (a directory) of System Support Maps (SSMs). Treat each Responsibility node as the root of a graph comprised of all the nodes that are linked to it in the SSM to which it belongs. Traverse that graph, attaching to each node the rlabel that uniquely identifies the root Responsibility.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing</t>
+  </si>
+  <si>
+    <t>add_rlabels_to_SSMs.py indir outdir [use_full_filename] [undir]</t>
+  </si>
+  <si>
+    <t>CMs_to_3cols</t>
+  </si>
+  <si>
+    <t>CMs_to_3cols.py cm_dir output_dir [min_val]</t>
+  </si>
+  <si>
+    <t>Miscellaneous scripts</t>
+  </si>
+  <si>
+    <t>get_maps_by_version</t>
+  </si>
+  <si>
+    <t>get_maps_by_version.py version output_directory</t>
+  </si>
+  <si>
+    <t>get_NY_maps_with_demo</t>
+  </si>
+  <si>
+    <t>get_NY_maps_with_demo.py output_directory</t>
+  </si>
+  <si>
+    <t>get_reg_info</t>
+  </si>
+  <si>
+    <t>get_reg_info in_dir out_fname</t>
+  </si>
+  <si>
+    <t>get_ssm_demographics</t>
+  </si>
+  <si>
+    <t>get_ssm_demographics.py in_dir</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-add_codes_to_ssms.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/add_rlabels_to_SSMs.py</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-create_code_matrices.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-get_maps_by_version.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-get_mental_maps.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-text2JSON.md</t>
+  </si>
+  <si>
+    <t>https://ssm.cloudapps.unc.edu/</t>
+  </si>
+  <si>
+    <t>https://sc.unc.edu/stevec/ssm.git</t>
+  </si>
+  <si>
+    <t>"Review and Next Steps" page text assumes "Finish" button?**</t>
+  </si>
+  <si>
+    <t>yes: Onyen-based  Shibboleth  connection with added restrictions</t>
+  </si>
+  <si>
+    <t>Ruchir Karmali. Access also available to Steve Chall, Kristen Hassmiller Lich, and Mikeala Roberson. All other access prohibited.</t>
+  </si>
+  <si>
+    <t>ssm variant that implements IRB-mandated "Level II Data Security" requirements for School of Public Health doctoral student Ruchir Karmali's research. Uses Shibboleth and middleware functionality provided by the related but not identical ITS Cloudapps (cloudapps@unc.edu) and ITS IdM (Identity Management: idman@unc.edu) groups to restrict password access to four Onyen-equipped users: Steve Chall (stevec), Kristen Hassmiller Lich (hassmill), Ruchir (rkarmali), and research assistant Mikeala Roberson (mikeala). Note that this version of ssm has the back end disabled for security purposes: all fetching and saving of ssm .json files must be done from and to the local (presumably IRB-approved secure) machine.</t>
+  </si>
+  <si>
+    <t>Documents, videos, etc. developed to support use?</t>
+  </si>
+  <si>
+    <t>ssm-wizard for Family Planning project/Title X. Based on http://syssci.renci.org/ssm-wizard/?module=TitleVWorkforce but includes custom text and demographic questions.Checkboxes with optional text entry response completion  for "Role" and "Workplace setting".</t>
+  </si>
+  <si>
+    <t>monodirectionalize_SSM_edges.py indir outdir</t>
+  </si>
+  <si>
+    <t>monodirectionalize_SSM_edges</t>
+  </si>
+  <si>
+    <t>Reads in a directory of code matrices (CMs). Outputs a directory of "3cols," which are 2D arrays, each arranged in three columns, thusly:
+    from    to   value
+where "from" and "to" are codes, and "value" is the number of edges in the originating set of SSMs that go from "from" to "to." In each 3cols file output there is a row for each element in its corresponding CM.</t>
+  </si>
+  <si>
+    <t>Read in a set (a directory) of System Support Maps (SSMs). For each map, create another map that's identical except that the direction of all the inward-pointing arrows is flipped so that all arrows point outwards. Assumption: that all arrows from Role and Responsibility nodes point outward, and all other arrows point inward. Used as a precursor to add_rlabels_to_SSMs so that the rlabels are assigned correctly.</t>
+  </si>
+  <si>
+    <t>Retrieve and write as .json files all the system support maps (ssms) from the ssm database that have a "version" value in the "document" field that matches command line argument "version."</t>
+  </si>
+  <si>
+    <t>Retrieve and write as .json files all the system support maps (ssms) from the ssm database that have a "state" key in the "document" field and where the associated value is "NY".</t>
+  </si>
+  <si>
+    <t>Read a directory of ssms, write out their demographic info to a csv file called demographics.csv.</t>
+  </si>
+  <si>
+    <t>Get registration info for each user associated with one or more of a directory of system support maps.</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>First Name; Last Name; Role; Organizations's Title X affilation; Workplace Setting; State; County or equivalent; City; Zip code; Reason for using the System Support Mapper</t>
+  </si>
+  <si>
     <r>
-      <t>Assumes that the files in the two directories follow this naming convention: 1) (cblm) coded binary link matrix: "</t>
+      <t>For each System Support Map (plus a summary CM that adds all the CMs for all SSMs in a project) we create a Code Matrix. The rows and columns are named with the project codes that have been generated. The matrix elements are integers that show, for element[i, j], how often a node that has been associated with code i is connected to a node that has been associated with code j. Assumes that the files in the two directories follow this naming convention: 1) (cblm) coded binary link matrix: "</t>
     </r>
     <r>
       <rPr>
@@ -314,358 +662,11 @@
       <t xml:space="preserve"> is a string that may or may not be constructed according to a convention defined in https://github.com/steve9000gi/extractMaps/blob/master/README.md.</t>
     </r>
   </si>
-  <si>
-    <t>Is it easier to put the demog survey in as a separate webpage, which when complete passes info to the wizard (advantage being that we can use the wizard site infrastructure (passing a new yaml, and a project specific demog survey and potentially project specific drop down lists, etc).</t>
-  </si>
-  <si>
-    <t>do now</t>
-  </si>
-  <si>
-    <t>Is it easy to name the .json files geog_firstPartEmail_SSMID_role.json</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>**The "Finish" button has been hidden in an effort to improve the user experience. Problem: Now, any post-wizard user changes to the map are not preserved.</t>
-  </si>
-  <si>
-    <t>Green fill means that presence or absence of drop-down lists in this version corresponds to text (no mention of drop-down lists if there aren't any).</t>
-  </si>
-  <si>
-    <t>Gray fill means this website is decommissioned, i.e., the user can't see it and is instead redirected to another website.</t>
-  </si>
-  <si>
-    <t>* Should the Qualtrics surveys be removed? Who's using them? 2017/06/05: we're keeping them and adding one for TitleX/Family Planning.</t>
-  </si>
-  <si>
-    <t>CYSHCN: fixed 2017/06/13</t>
-  </si>
-  <si>
-    <t>Demographic questions?</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>state; county/municipality; race;  Hispanic?; language;  child's age; insurance; health conditions</t>
-  </si>
-  <si>
-    <t>position; grade[s]; age range; years at school;  race/ethnicity; school location</t>
-  </si>
-  <si>
-    <t>Wizard prototype (maintained for backwards compatibility). Identical to ssm-wizard-d/?module=CaregiversOfCYSHCN from the user's viewpoint. Decommissioned 2017/06/13: url redirects to http://syssci.renci.org/ssm-wizard-d/?module=CaregiversOfCYSHCN.</t>
-  </si>
-  <si>
-    <t>NA (decommissioned)</t>
-  </si>
-  <si>
-    <t>Documents</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm/blob/master/SSM-websites-and-software.xlsx</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm/blob/master/SSM_Processing_Sequence.txt</t>
-  </si>
-  <si>
-    <t>This spreadsheet</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/sort/blob/master/Editing_Sorted_SSM_Documents.docx</t>
-  </si>
-  <si>
-    <t>Tips for manually editing sorted text items while maximizing the likelihood of the results being processable.</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/sort/blob/master/File_Formats_for_the_Sort_Segment_of_the_System_Support_Mapping_Processing_Sequence.docx</t>
-  </si>
-  <si>
-    <t>Details of the various sort file formats with emphasis on .json.</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm/blob/master/README.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/binary-link-matrix/blob/master/README.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/sort/blob/master/README.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/AddCodesToBLM/blob/master/README.md</t>
-  </si>
-  <si>
-    <t>Also the README.md files in the various SSM-related GitHub repos:</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/extractMaps/blob/master/README.md</t>
-  </si>
-  <si>
-    <t>Text-only example runthrough : SSMs -&gt; BLMS -&gt; sort -&gt; CBLM -&gt; CM and CPM</t>
-  </si>
-  <si>
-    <t>8/10/2017 for all SSM Wizard versions:</t>
-  </si>
-  <si>
-    <t>Restore hidden ""Finish" button as "Save" (doesn't close wizard)</t>
-  </si>
-  <si>
-    <t>Fix Minimize</t>
-  </si>
-  <si>
-    <t>Enforce limits on zoom and translate</t>
-  </si>
-  <si>
-    <t>Fix completions (elements of completions objects should be arrays)</t>
-  </si>
-  <si>
-    <t>Add wizard type (e.g., TitleX or TitleV), version number, and timestamp to source and to SSM json output</t>
-  </si>
-  <si>
-    <t>http://syssci.renci.org/ssm-wizard-TitleX</t>
-  </si>
-  <si>
-    <t>generic</t>
-  </si>
-  <si>
-    <t>"Finish" converted to "Save"</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm/tree/wizard-TitleX</t>
-  </si>
-  <si>
-    <t>http://syssci.renci.org/ssm-wizard-TitleV</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm/tree/wizard-TitleV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In use? </t>
-  </si>
-  <si>
-    <t>For "Role" only</t>
-  </si>
-  <si>
-    <t>ssm-wizard for Maternal and Child Health/Title V. Based on http://syssci.renci.org/ssm-wizard/?module=TitleVWorkforce but includes custom text and demographic questions. No text entry response dropdown completions lists.</t>
-  </si>
-  <si>
-    <t>Dropdown completions lists for text entry</t>
-  </si>
-  <si>
-    <t>ALL (done for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
-  </si>
-  <si>
-    <t>ALL (done for ssm-wizard-TitleX)</t>
-  </si>
-  <si>
-    <t>ALL (type only displayed for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
-  </si>
-  <si>
-    <t>8/15/2017:</t>
-  </si>
-  <si>
-    <t>Add wizard version (e.g., TitleX or TitleV) and timestamp to source and to SSM json output</t>
-  </si>
-  <si>
-    <t>done for ssm-wizard-TitleX, ssm-wizard-TitleV, ssm, ssm-wizard, ssm-wizard-d)</t>
-  </si>
-  <si>
-    <t>not done: mental, beh</t>
-  </si>
-  <si>
-    <t>In use by…</t>
-  </si>
-  <si>
-    <t>Fill in who is currently using each website (over time)</t>
-  </si>
-  <si>
-    <t>Fill in all docs, videos etc that support use of each version of the wizard</t>
-  </si>
-  <si>
-    <t>UIC doctoral student Kevin Borrup's "Roles in Mental Health Care within Schools in Connecticut Research Study."</t>
-  </si>
-  <si>
-    <t>Detailed guide with screenshots for parents/caregivers of CYSHN; https://www.youtube.com/channel/UCFTWoJ1iXFTqrq-62RZ68hA</t>
-  </si>
-  <si>
-    <t>done for http://syssci.renci.org/ssm-wizard-TitleX</t>
-  </si>
-  <si>
-    <t>look into [probably not. Would require passing data between websites.]</t>
-  </si>
-  <si>
-    <t>if easy [possible but not easy: requires JSON data extraction within PostgreSQL]</t>
-  </si>
-  <si>
-    <t>youtube site with instructions for the Title V SSM Wizard</t>
-  </si>
-  <si>
-    <t> https://www.youtube.com/channel/UCFTWoJ1iXFTqrq-62RZ68hA</t>
-  </si>
-  <si>
-    <t>Deanna Befus</t>
-  </si>
-  <si>
-    <t>NY State DOH caregivers</t>
-  </si>
-  <si>
-    <t>NMCHWDC Workforce; NY State DOH workforce</t>
-  </si>
-  <si>
-    <t>Larissa Calancie: Title V NMCHWDC</t>
-  </si>
-  <si>
-    <t>decommissioned</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>"ssm"</t>
-  </si>
-  <si>
-    <t>"ssm-wizard-TitleV"</t>
-  </si>
-  <si>
-    <t>"ssm-wizard-d (/?module=CaregiversOfCYSHCN)"</t>
-  </si>
-  <si>
-    <t>"ssm-wizard-TitleX"</t>
-  </si>
-  <si>
-    <t>"ssm-wizard"</t>
-  </si>
-  <si>
-    <t>Version/Timestamp</t>
-  </si>
-  <si>
-    <t>Draft TitleX questions need to be updated. Also awaiting general review of user interface.</t>
-  </si>
-  <si>
-    <t>add_rlabels_to_SSMs</t>
-  </si>
-  <si>
-    <t>add_rlabels_to_SSMs.py. An "rlabel" is a string that uniquely identifies a Responsibility node in the context of a set (a directory) of System Support Maps (SSMs). Treat each Responsibility node as the root of a graph comprised of all the nodes that are linked to it in the SSM to which it belongs. Traverse that graph, attaching to each node the rlabel that uniquely identifies the root Responsibility.</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm_processing</t>
-  </si>
-  <si>
-    <t>add_rlabels_to_SSMs.py indir outdir [use_full_filename] [undir]</t>
-  </si>
-  <si>
-    <t>CMs_to_3cols</t>
-  </si>
-  <si>
-    <t>CMs_to_3cols.py cm_dir output_dir [min_val]</t>
-  </si>
-  <si>
-    <t>Miscellaneous scripts</t>
-  </si>
-  <si>
-    <t>get_maps_by_version</t>
-  </si>
-  <si>
-    <t>get_maps_by_version.py version output_directory</t>
-  </si>
-  <si>
-    <t>get_NY_maps_with_demo</t>
-  </si>
-  <si>
-    <t>get_NY_maps_with_demo.py output_directory</t>
-  </si>
-  <si>
-    <t>get_reg_info</t>
-  </si>
-  <si>
-    <t>get_reg_info in_dir out_fname</t>
-  </si>
-  <si>
-    <t>get_ssm_demographics</t>
-  </si>
-  <si>
-    <t>get_ssm_demographics.py in_dir</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-add_codes_to_ssms.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm_processing/blob/master/add_rlabels_to_SSMs.py</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-create_code_matrices.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-get_maps_by_version.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-get_mental_maps.md</t>
-  </si>
-  <si>
-    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-text2JSON.md</t>
-  </si>
-  <si>
-    <t>https://ssm.cloudapps.unc.edu/</t>
-  </si>
-  <si>
-    <t>https://sc.unc.edu/stevec/ssm.git</t>
-  </si>
-  <si>
-    <t>"Review and Next Steps" page text assumes "Finish" button?**</t>
-  </si>
-  <si>
-    <t>yes: Onyen-based  Shibboleth  connection with added restrictions</t>
-  </si>
-  <si>
-    <t>Ruchir Karmali. Access also available to Steve Chall, Kristen Hassmiller Lich, and Mikeala Roberson. All other access prohibited.</t>
-  </si>
-  <si>
-    <t>ssm variant that implements IRB-mandated "Level II Data Security" requirements for School of Public Health doctoral student Ruchir Karmali's research. Uses Shibboleth and middleware functionality provided by the related but not identical ITS Cloudapps (cloudapps@unc.edu) and ITS IdM (Identity Management: idman@unc.edu) groups to restrict password access to four Onyen-equipped users: Steve Chall (stevec), Kristen Hassmiller Lich (hassmill), Ruchir (rkarmali), and research assistant Mikeala Roberson (mikeala). Note that this version of ssm has the back end disabled for security purposes: all fetching and saving of ssm .json files must be done from and to the local (presumably IRB-approved secure) machine.</t>
-  </si>
-  <si>
-    <t>Documents, videos, etc. developed to support use?</t>
-  </si>
-  <si>
-    <t>ssm-wizard for Family Planning project/Title X. Based on http://syssci.renci.org/ssm-wizard/?module=TitleVWorkforce but includes custom text and demographic questions.Checkboxes with optional text entry response completion  for "Role" and "Workplace setting".</t>
-  </si>
-  <si>
-    <t>monodirectionalize_SSM_edges.py indir outdir</t>
-  </si>
-  <si>
-    <t>monodirectionalize_SSM_edges</t>
-  </si>
-  <si>
-    <t>Reads in a directory of code matrices (CMs). Outputs a directory of "3cols," which are 2D arrays, each arranged in three columns, thusly:
-    from    to   value
-where "from" and "to" are codes, and "value" is the number of edges in the originating set of SSMs that go from "from" to "to." In each 3cols file output there is a row for each element in its corresponding CM.</t>
-  </si>
-  <si>
-    <t>Read in a set (a directory) of System Support Maps (SSMs). For each map, create another map that's identical except that the direction of all the inward-pointing arrows is flipped so that all arrows point outwards. Assumption: that all arrows from Role and Responsibility nodes point outward, and all other arrows point inward. Used as a precursor to add_rlabels_to_SSMs so that the rlabels are assigned correctly.</t>
-  </si>
-  <si>
-    <t>Retrieve and write as .json files all the system support maps (ssms) from the ssm database that have a "version" value in the "document" field that matches command line argument "version."</t>
-  </si>
-  <si>
-    <t>Retrieve and write as .json files all the system support maps (ssms) from the ssm database that have a "state" key in the "document" field and where the associated value is "NY".</t>
-  </si>
-  <si>
-    <t>Read a directory of ssms, write out their demographic info to a csv file called demographics.csv.</t>
-  </si>
-  <si>
-    <t>Get registration info for each user associated with one or more of a directory of system support maps.</t>
-  </si>
-  <si>
-    <t>]</t>
-  </si>
-  <si>
-    <t>First Name; Last Name; Role; Organizations's Title X affilation; Workplace Setting; State; County or equivalent; City; Zip code; Reason for using the System Support Mapper</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -928,7 +929,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1111,6 +1112,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="30" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="30" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1647,11 +1654,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1745,7 +1752,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>22</v>
@@ -1767,7 +1774,7 @@
         <v>44</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>23</v>
@@ -1799,7 +1806,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="2:8" s="24" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" s="24" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="B12" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1808,10 +1815,10 @@
         <v>55</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>35</v>
@@ -1833,7 +1840,7 @@
         <v>37</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>36</v>
@@ -1848,16 +1855,16 @@
         <v>8</v>
       </c>
       <c r="C14" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="F14" s="23" t="s">
         <v>151</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>152</v>
       </c>
       <c r="G14" s="21" t="s">
         <v>40</v>
@@ -1869,16 +1876,16 @@
         <v>9</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>40</v>
@@ -1890,16 +1897,16 @@
         <v>10</v>
       </c>
       <c r="C16" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>153</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>154</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>40</v>
@@ -1908,7 +1915,7 @@
     <row r="17" spans="2:7" s="57" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="16"/>
       <c r="C17" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>1</v>
@@ -1928,16 +1935,16 @@
         <v>11</v>
       </c>
       <c r="C18" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>156</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>157</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>40</v>
@@ -1948,16 +1955,16 @@
         <v>12</v>
       </c>
       <c r="C19" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>158</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>159</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>40</v>
@@ -1968,16 +1975,16 @@
         <v>13</v>
       </c>
       <c r="C20" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>160</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>161</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>40</v>
@@ -1988,16 +1995,16 @@
         <v>14</v>
       </c>
       <c r="C21" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>162</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>163</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>40</v>
@@ -2005,7 +2012,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B22" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2021,15 +2028,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O217"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -2076,34 +2083,34 @@
         <v>1</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" s="48" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H2" s="48" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J2" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K2" s="48" t="s">
         <v>63</v>
       </c>
       <c r="L2" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M2" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="84" x14ac:dyDescent="0.2">
@@ -2117,7 +2124,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>29</v>
@@ -2126,7 +2133,7 @@
         <v>69</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>13</v>
@@ -2141,7 +2148,7 @@
         <v>58</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>61</v>
@@ -2152,7 +2159,7 @@
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="66" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -2166,7 +2173,7 @@
         <v>69</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>13</v>
@@ -2187,10 +2194,10 @@
         <v>61</v>
       </c>
       <c r="N4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4" s="35" t="s">
         <v>78</v>
-      </c>
-      <c r="O4" s="35" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="42" x14ac:dyDescent="0.2">
@@ -2198,7 +2205,7 @@
         <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="66" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -2210,13 +2217,13 @@
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J5" s="33" t="s">
         <v>59</v>
@@ -2225,7 +2232,7 @@
         <v>59</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M5" s="11" t="s">
         <v>13</v>
@@ -2236,7 +2243,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="66" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2248,13 +2255,13 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J6" s="33" t="s">
         <v>58</v>
@@ -2263,7 +2270,7 @@
         <v>60</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>13</v>
@@ -2278,7 +2285,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="60" t="s">
@@ -2288,13 +2295,13 @@
         <v>14</v>
       </c>
       <c r="G7" s="54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H7" s="37" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>59</v>
@@ -2307,10 +2314,10 @@
         <v>13</v>
       </c>
       <c r="N7" s="62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O7" s="64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="126" x14ac:dyDescent="0.2">
@@ -2336,16 +2343,16 @@
         <v>13</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>59</v>
       </c>
       <c r="L8" s="50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>13</v>
@@ -2358,7 +2365,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="66" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2372,13 +2379,13 @@
         <v>13</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J9" s="33" t="s">
         <v>58</v>
@@ -2398,15 +2405,15 @@
         <f>A8+1</f>
         <v>7</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>109</v>
+      <c r="B10" s="66" t="s">
+        <v>108</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>14</v>
@@ -2416,19 +2423,19 @@
         <v>13</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J10" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="M10" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="L10" s="50" t="s">
-        <v>145</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.2">
@@ -2437,14 +2444,14 @@
         <v>8</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>14</v>
@@ -2454,7 +2461,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J11" s="33" t="s">
         <v>58</v>
@@ -2463,10 +2470,10 @@
         <v>60</v>
       </c>
       <c r="L11" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="126" x14ac:dyDescent="0.2">
@@ -2524,7 +2531,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>14</v>
@@ -2546,24 +2553,24 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="252" x14ac:dyDescent="0.2">
-      <c r="B14" s="58" t="s">
-        <v>170</v>
+      <c r="B14" s="67" t="s">
+        <v>169</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>61</v>
@@ -3368,19 +3375,20 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B11" r:id="rId6"/>
-    <hyperlink ref="B12" r:id="rId7"/>
-    <hyperlink ref="B13" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="B14" r:id="rId11"/>
-    <hyperlink ref="E14" r:id="rId12"/>
-    <hyperlink ref="E3:E14" r:id="rId13" display="https://github.com/steve9000gi/ssm/tree/master"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E3:E14" r:id="rId13" display="https://github.com/steve9000gi/ssm/tree/master" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="B4" r:id="rId14" xr:uid="{F7B83C6B-97D2-0D4E-95A9-DFA948946C9D}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup scale="35" fitToHeight="2" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3393,7 +3401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3418,7 +3426,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>65</v>
@@ -3427,12 +3435,12 @@
         <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>68</v>
@@ -3443,7 +3451,7 @@
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>71</v>
@@ -3454,31 +3462,31 @@
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3486,12 +3494,12 @@
         <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" t="s">
         <v>67</v>
@@ -3499,7 +3507,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
@@ -3507,37 +3515,37 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3549,12 +3557,12 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3569,7 +3577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3584,7 +3592,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.2">
@@ -3597,107 +3605,107 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
         <v>94</v>
-      </c>
-      <c r="B6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A20" r:id="rId1"/>
+    <hyperlink ref="A20" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3710,7 +3718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
new info for rcoding, etc.
</commit_message>
<xml_diff>
--- a/SSM-websites-and-software.xlsx
+++ b/SSM-websites-and-software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevec/ssm-documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D60BE04-8A72-D141-AA91-455D0854E5B0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AC09A0E4-9969-B640-93E1-7D14C2DBD4B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37360" yWindow="720" windowWidth="36540" windowHeight="21760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38500" yWindow="0" windowWidth="37980" windowHeight="22700" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataProcSeqAndProcesses" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="204">
   <si>
     <t>URL</t>
   </si>
@@ -662,6 +662,54 @@
       <t xml:space="preserve"> is a string that may or may not be constructed according to a convention defined in https://github.com/steve9000gi/extractMaps/blob/master/README.md.</t>
     </r>
   </si>
+  <si>
+    <t>rlabels2rcodes.py</t>
+  </si>
+  <si>
+    <t>rlabels2rcodes.py path/to/sorted_resp_file rlabeled_ssm_dir rcoded_ssm_dir</t>
+  </si>
+  <si>
+    <t>Assumes that there exists, for a directory of System Support Maps (SSMs), a JSON file that contains the all Responsibility node text items from those SSMs, sorted by code, and with the same format as output by the "sort"  online utility (see https://github.com/steve9000gi/sort). Args: sorted_resp_file: file of responsibility node texts, sorted by codes rlabeled_ssm_dir: A directory (required to exist) that contains a set of rlabeled SSMs.rcoded_ssm_dir: an output directory of SSMs, identical to rlabeled_ssm_dir except that every rlabel in every SSM has been replaced by its corresponding rcode.</t>
+  </si>
+  <si>
+    <t>http://syssci.renci.org/sort-rcode/</t>
+  </si>
+  <si>
+    <t>Like sort except with additional constraints to support sorting rcoded lists of text items, e.g., the first item to be dropped into a box has its rcode appended to the box title (code). If the item has multiple rcodes, the user is asked to choose one. Only one rcode per box is permitted.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/tree/sort-rcode</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/blob/sort-rcode/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/force-directed-map</t>
+  </si>
+  <si>
+    <t>y?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>OLDER</t>
+  </si>
+  <si>
+    <t>​New bug for sort and sort-rcoded websites: when editing text boxes, the text is invisible.</t>
+  </si>
+  <si>
+    <t>Need to write CMs_to_4cols.py script to extract rcodes from text items and insert into 4th column.</t>
+  </si>
+  <si>
+    <t>All the SSM websites should be ported to secure https://syssci-1.renci.org from non-secure http://syssci.renci.org​. This would require that all subsidiary JavaScript library links be to secure (https) sites as well.</t>
+  </si>
+  <si>
+    <t>Move all d3.js from v3 to v4.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm_processing/blob/master/README-rlabels2rcodes.MD</t>
+  </si>
 </sst>
 </file>
 
@@ -670,7 +718,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -766,6 +814,13 @@
       <strike/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -929,7 +984,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1102,6 +1157,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1114,11 +1175,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="30" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="30" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="60">
@@ -1655,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H22"/>
+  <dimension ref="B1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2010,8 +2087,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B22" s="26" t="s">
+    <row r="22" spans="2:7" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="20">
+        <v>14</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B23" s="26" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2032,17 +2129,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O217"/>
+  <dimension ref="A1:O218"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="56.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="56.83203125" style="62" customWidth="1"/>
     <col min="3" max="3" width="78.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="41.83203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="38" style="12" customWidth="1"/>
@@ -2117,7 +2214,7 @@
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2159,7 +2256,7 @@
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -2202,10 +2299,10 @@
     </row>
     <row r="5" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
-        <f t="shared" ref="A5:A13" si="0">A4+1</f>
+        <f t="shared" ref="A5:A12" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="32" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -2243,7 +2340,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2300,7 +2397,7 @@
       <c r="H7" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I7" s="71" t="s">
         <v>86</v>
       </c>
       <c r="J7" s="33" t="s">
@@ -2313,10 +2410,10 @@
       <c r="M7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="62" t="s">
+      <c r="N7" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="O7" s="64" t="s">
+      <c r="O7" s="66" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2342,7 +2439,7 @@
       <c r="H8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="70" t="s">
         <v>83</v>
       </c>
       <c r="J8" s="33" t="s">
@@ -2357,15 +2454,15 @@
       <c r="M8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="63"/>
-      <c r="O8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="67"/>
     </row>
     <row r="9" spans="1:15" ht="126" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2376,7 +2473,7 @@
         <v>34</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>128</v>
@@ -2384,7 +2481,7 @@
       <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="70" t="s">
         <v>84</v>
       </c>
       <c r="J9" s="33" t="s">
@@ -2405,7 +2502,7 @@
         <f>A8+1</f>
         <v>7</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="32" t="s">
         <v>108</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -2416,13 +2513,13 @@
         <v>111</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="70" t="s">
         <v>186</v>
       </c>
       <c r="J10" s="46" t="s">
@@ -2454,13 +2551,13 @@
         <v>113</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="70" t="s">
         <v>147</v>
       </c>
       <c r="J11" s="33" t="s">
@@ -2488,10 +2585,10 @@
         <v>57</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="E12" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="9" t="s">
         <v>14</v>
@@ -2499,7 +2596,7 @@
       <c r="I12" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="J12" s="68" t="s">
         <v>61</v>
       </c>
       <c r="K12" s="7" t="s">
@@ -2512,10 +2609,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="84" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" s="63" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>A11+1</f>
+        <v>9</v>
       </c>
       <c r="B13" s="58" t="s">
         <v>15</v>
@@ -2523,7 +2620,9 @@
       <c r="C13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="69" t="s">
+        <v>194</v>
+      </c>
       <c r="E13" s="45" t="s">
         <v>24</v>
       </c>
@@ -2539,7 +2638,7 @@
       <c r="I13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="68" t="s">
         <v>61</v>
       </c>
       <c r="K13" s="7" t="s">
@@ -2552,45 +2651,81 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="252" x14ac:dyDescent="0.2">
-      <c r="B14" s="67" t="s">
-        <v>169</v>
+    <row r="14" spans="1:15" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <f>A12+1</f>
+        <v>10</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>191</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="45" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="J14" s="68" t="s">
         <v>61</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>61</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="M14" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+    <row r="15" spans="1:15" ht="252" x14ac:dyDescent="0.2">
+      <c r="B15" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H15" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="24" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H24" s="12"/>
@@ -3367,6 +3502,10 @@
     <row r="217" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H217" s="12"/>
       <c r="I217" s="12"/>
+    </row>
+    <row r="218" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H218" s="12"/>
+      <c r="I218" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3382,13 +3521,17 @@
     <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
     <hyperlink ref="B11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
     <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="B13" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B14" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
     <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="B14" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="E3:E14" r:id="rId13" display="https://github.com/steve9000gi/ssm/tree/master" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="B4" r:id="rId14" xr:uid="{F7B83C6B-97D2-0D4E-95A9-DFA948946C9D}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="B4" r:id="rId13" xr:uid="{F7B83C6B-97D2-0D4E-95A9-DFA948946C9D}"/>
+    <hyperlink ref="B3" r:id="rId14" xr:uid="{67083D96-62FE-344E-9922-624B277518DA}"/>
+    <hyperlink ref="B13" r:id="rId15" xr:uid="{F198A134-90F3-6840-9721-93E89E1F5E76}"/>
+    <hyperlink ref="E13" r:id="rId16" display="https://github.com/steve9000gi/ssm/tree/master" xr:uid="{7A7C4B65-94FB-5C41-B7CC-34A75AA19368}"/>
+    <hyperlink ref="E14" r:id="rId17" xr:uid="{AE1BF42F-947C-C04A-885F-122BFA39BE2E}"/>
+    <hyperlink ref="D13" r:id="rId18" xr:uid="{1BF54931-1FC0-C34F-89D9-5243D68CED6B}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup scale="35" fitToHeight="2" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3402,10 +3545,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3415,153 +3558,200 @@
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30"/>
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="73">
+        <v>43333</v>
+      </c>
+      <c r="B1" s="51"/>
+    </row>
+    <row r="2" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="74" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="75"/>
+    </row>
+    <row r="3" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="75"/>
+    </row>
+    <row r="4" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="75"/>
+    </row>
+    <row r="5" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="75"/>
+    </row>
+    <row r="6" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="75"/>
+    </row>
+    <row r="7" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="75"/>
+    </row>
+    <row r="8" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="74" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="75"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="30"/>
+      <c r="B14" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C14" s="27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B15" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C15" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B16" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B17" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+    <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B18" s="29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B19" s="29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="44" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="44" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="29" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="29" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="29" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="29" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="29" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C27" s="47" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="52" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C28" s="47" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="51" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="51" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+    <row r="31" spans="1:4" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B31" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C31" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D31" s="42" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
-      <c r="B19" s="55">
+    <row r="32" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="42"/>
+      <c r="B32" s="55">
         <v>42963</v>
       </c>
-      <c r="D19" s="42"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="29" t="s">
+      <c r="D32" s="42"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="29" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="29" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="29" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3578,10 +3768,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3695,17 +3885,22 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="56" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="42" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A20" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>